<commit_message>
DAY23 - DB COMMIT
</commit_message>
<xml_diff>
--- a/First_Project/ORACLEDB/SHOPPING_MALL_DB_PRACTICE.xlsx
+++ b/First_Project/ORACLEDB/SHOPPING_MALL_DB_PRACTICE.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TJ-BU-708-P11\git\first_java\First_Project\ORACLEDB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804D16CD-07E9-4727-9141-A306C6263D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="시트1" sheetId="1" r:id="rId4"/>
+    <sheet name="시트1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -262,26 +271,36 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -289,7 +308,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -299,41 +318,47 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -523,466 +548,486 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B1:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="14.13"/>
-    <col customWidth="1" min="3" max="3" width="9.0"/>
-    <col customWidth="1" min="4" max="4" width="10.13"/>
-    <col customWidth="1" min="6" max="6" width="17.25"/>
-    <col customWidth="1" min="7" max="7" width="9.0"/>
-    <col customWidth="1" min="8" max="8" width="10.13"/>
-    <col customWidth="1" min="9" max="9" width="16.13"/>
-    <col customWidth="1" min="11" max="11" width="22.88"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5703125" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5703125" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="K1" s="1" t="s">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="K2" s="1" t="s">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="L4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="1"/>
+      <c r="L5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6">
-      <c r="B6" s="3" t="s">
+      <c r="N5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="K6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7">
-      <c r="B7" s="3" t="s">
+      <c r="N6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="N9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="O9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="Q9" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="L11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="O13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="Q13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="3" t="s">
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="E14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="Q15" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L18" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L19" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L22" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L23" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="F16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="F17" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="K18" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="K19" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="K21" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="K22" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="K23" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25">
-      <c r="K25" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="K26" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="K28" s="3" t="s">
+    </row>
+    <row r="28" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L28" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29">
-      <c r="K29" s="3" t="s">
+    <row r="29" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L29" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31">
-      <c r="K31" s="3" t="s">
+    <row r="31" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L31" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32">
-      <c r="K32" s="3" t="s">
+    <row r="32" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="L32" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34">
-      <c r="K34" s="3" t="s">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L34" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35">
-      <c r="K35" s="3" t="s">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L35" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37">
-      <c r="K37" s="3" t="s">
+    <row r="37" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L37" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38">
-      <c r="K38" s="3" t="s">
+    <row r="38" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L38" s="2" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="G4:J4"/>
     <mergeCell ref="B4:E4"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>